<commit_message>
revision submitted to ESCO
</commit_message>
<xml_diff>
--- a/word_revision/Table2.xlsx
+++ b/word_revision/Table2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\docs\manuscripts\sgdepth_manu\word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\docs\manuscripts\sgdepth_manu\word_revision\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -130,6 +130,22 @@
   </si>
   <si>
     <r>
+      <t>Segment</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -145,30 +161,14 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Summary of seagrass depth estimates (m) for each segment in Fig. 4. Whole segment estimates and prediction intervals were obtained from a single point estimate that included all seagrass depth data for the segment.  Mean, standard error, standard deviation, minimum, and maximum values are for multiple grid points within each segment in Fig. 4. Mean and standard error estimates were from intercept-only models that included Gaussian correlation structures to account for spatial dependencies between points</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Segment</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>a</t>
+      <t xml:space="preserve"> Summary of seagrass depth estimates (m) for each segment in Fig. 4 and the year indicated in Table 1. Whole segment estimates and prediction intervals were obtained from a single point estimate that included all seagrass depth data for the segment.  Mean, standard error, standard deviation, minimum, and maximum values are for multiple grid points within each segment in Fig. 4. Mean and standard error estimates were from intercept-only models that included Gaussian correlation structures to account for spatial dependencies between points</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,13 +346,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -448,6 +448,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -483,6 +500,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -638,7 +672,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,20 +684,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="A1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -1153,16 +1187,16 @@
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>

</xml_diff>